<commit_message>
Jogo simples acabado, falta fazer limpeza
</commit_message>
<xml_diff>
--- a/Mapa 1.xlsx
+++ b/Mapa 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eng. Informatica\2017-2018\SO\Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eng, Informatica\2017-2018\SO\SO-Trabalho1-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -723,19 +723,31 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -756,23 +768,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1199,10 +1199,10 @@
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="23"/>
-      <c r="O8" s="47" t="s">
+      <c r="O8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="48"/>
+      <c r="P8" s="52"/>
       <c r="Q8" s="8" t="s">
         <v>19</v>
       </c>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="9" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="25"/>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="45" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="37" t="s">
@@ -1249,12 +1249,12 @@
     </row>
     <row r="10" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="25"/>
-      <c r="G10" s="40"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="34"/>
       <c r="I10" s="31"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="49" t="s">
+      <c r="L10" s="53" t="s">
         <v>1</v>
       </c>
       <c r="M10" s="5"/>
@@ -1277,18 +1277,18 @@
     </row>
     <row r="11" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="25"/>
-      <c r="G11" s="54"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="33"/>
       <c r="I11" s="32"/>
       <c r="J11" s="17"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="41" t="s">
+      <c r="L11" s="53"/>
+      <c r="M11" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="43"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="48"/>
       <c r="Q11" s="6"/>
       <c r="U11" s="35" t="s">
         <v>6</v>
@@ -1298,21 +1298,21 @@
       </c>
     </row>
     <row r="12" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="53"/>
-      <c r="G12" s="55" t="s">
+      <c r="F12" s="42"/>
+      <c r="G12" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="56"/>
+      <c r="H12" s="44"/>
       <c r="I12" s="20" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="20"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="46"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="50"/>
       <c r="Q12" s="6"/>
       <c r="U12" s="35" t="s">
         <v>18</v>
@@ -1323,12 +1323,12 @@
     </row>
     <row r="13" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="4"/>
-      <c r="G13" s="51"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="9"/>
       <c r="I13" s="36"/>
       <c r="J13" s="36"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="50"/>
+      <c r="L13" s="54"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="6"/>
@@ -1350,13 +1350,13 @@
       <c r="I14" s="58"/>
       <c r="J14" s="58"/>
       <c r="K14" s="59"/>
-      <c r="L14" s="42" t="s">
+      <c r="L14" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="43"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="48"/>
       <c r="Q14" s="6"/>
       <c r="U14" s="35" t="s">
         <v>20</v>
@@ -1378,11 +1378,11 @@
       <c r="I15" s="61"/>
       <c r="J15" s="61"/>
       <c r="K15" s="62"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="46"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="50"/>
       <c r="Q15" s="6"/>
       <c r="U15" s="35" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Todo o trabalho junto no main c, ainda resiste algo mal
</commit_message>
<xml_diff>
--- a/Mapa 1.xlsx
+++ b/Mapa 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eng, Informatica\2017-2018\SO\SO-Trabalho1-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eng. Informatica\2017-2018\SO\Trabalho1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -606,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -714,13 +714,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,6 +785,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1072,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:AI19"/>
+  <dimension ref="D1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:P15"/>
+    <sheetView tabSelected="1" topLeftCell="P5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1082,7 @@
     <col min="21" max="34" width="9.140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:34" x14ac:dyDescent="0.25">
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1098,12 +1095,12 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
     </row>
-    <row r="3" spans="6:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:34" x14ac:dyDescent="0.25">
       <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="6:35" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
         <v>23</v>
@@ -1120,7 +1117,7 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="6:35" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
@@ -1135,7 +1132,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="9"/>
@@ -1154,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G7" s="24"/>
       <c r="H7" s="7" t="s">
         <v>15</v>
@@ -1185,24 +1182,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="25"/>
       <c r="G8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="39"/>
+      <c r="I8" s="61"/>
       <c r="J8" s="18"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="23"/>
-      <c r="O8" s="51" t="s">
+      <c r="O8" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="52"/>
+      <c r="P8" s="50"/>
       <c r="Q8" s="8" t="s">
         <v>19</v>
       </c>
@@ -1212,19 +1209,26 @@
       <c r="W8" s="35">
         <v>2</v>
       </c>
-      <c r="AG8" s="35" t="s">
+      <c r="Y8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AI8">
+      <c r="AA8" s="35">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+    </row>
+    <row r="9" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="25"/>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="30" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="30">
@@ -1247,14 +1251,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="25"/>
-      <c r="G10" s="45"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="34"/>
       <c r="I10" s="31"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="53" t="s">
+      <c r="L10" s="51" t="s">
         <v>1</v>
       </c>
       <c r="M10" s="5"/>
@@ -1268,27 +1272,31 @@
       <c r="W10" s="35">
         <v>4</v>
       </c>
-      <c r="AC10" s="35" t="s">
+      <c r="Y10" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AE10" s="35">
+      <c r="AA10" s="35">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+    </row>
+    <row r="11" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="25"/>
-      <c r="G11" s="46"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="33"/>
       <c r="I11" s="32"/>
       <c r="J11" s="17"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="55" t="s">
+      <c r="L11" s="51"/>
+      <c r="M11" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="48"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="46"/>
       <c r="Q11" s="6"/>
       <c r="U11" s="35" t="s">
         <v>6</v>
@@ -1296,23 +1304,27 @@
       <c r="W11" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="42"/>
-      <c r="G12" s="43" t="s">
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+    </row>
+    <row r="12" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="40"/>
+      <c r="G12" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="44"/>
+      <c r="H12" s="42"/>
       <c r="I12" s="20" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="20"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="50"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="48"/>
       <c r="Q12" s="6"/>
       <c r="U12" s="35" t="s">
         <v>18</v>
@@ -1320,15 +1332,19 @@
       <c r="W12" s="35">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+    </row>
+    <row r="13" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="4"/>
-      <c r="G13" s="40"/>
+      <c r="G13" s="38"/>
       <c r="H13" s="9"/>
       <c r="I13" s="36"/>
       <c r="J13" s="36"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="54"/>
+      <c r="L13" s="52"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="6"/>
@@ -1340,23 +1356,27 @@
       <c r="W13" s="35">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="6:35" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+    </row>
+    <row r="14" spans="6:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="4"/>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="47" t="s">
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="48"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="46"/>
       <c r="Q14" s="6"/>
       <c r="U14" s="35" t="s">
         <v>20</v>
@@ -1364,25 +1384,29 @@
       <c r="W14" s="35">
         <v>8</v>
       </c>
-      <c r="AC14" s="35" t="s">
+      <c r="Y14" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AE14" s="35">
+      <c r="AA14" s="35">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="6:35" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+    </row>
+    <row r="15" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F15" s="4"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="50"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="48"/>
       <c r="Q15" s="6"/>
       <c r="U15" s="35" t="s">
         <v>1</v>
@@ -1391,7 +1415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="6:35" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1409,12 +1433,19 @@
       <c r="W16" s="35">
         <v>10</v>
       </c>
-      <c r="AG16" s="35" t="s">
+      <c r="Y16" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="AI16">
+      <c r="AA16" s="35">
         <v>19</v>
       </c>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
     </row>
     <row r="17" spans="12:27" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L17" s="4"/>

</xml_diff>

<commit_message>
Finalizado, uma bosta fedorenta, mas uma bosta acabada de cagar
</commit_message>
<xml_diff>
--- a/Mapa 1.xlsx
+++ b/Mapa 1.xlsx
@@ -732,6 +732,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -785,9 +788,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -1190,16 +1190,16 @@
       <c r="H8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="61"/>
+      <c r="I8" s="43"/>
       <c r="J8" s="18"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="23"/>
-      <c r="O8" s="49" t="s">
+      <c r="O8" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="50"/>
+      <c r="P8" s="51"/>
       <c r="Q8" s="8" t="s">
         <v>19</v>
       </c>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="9" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="25"/>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="44" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="30" t="s">
@@ -1253,12 +1253,12 @@
     </row>
     <row r="10" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="25"/>
-      <c r="G10" s="43"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="34"/>
       <c r="I10" s="31"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="51" t="s">
+      <c r="L10" s="52" t="s">
         <v>1</v>
       </c>
       <c r="M10" s="5"/>
@@ -1285,18 +1285,18 @@
     </row>
     <row r="11" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="25"/>
-      <c r="G11" s="44"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="33"/>
       <c r="I11" s="32"/>
       <c r="J11" s="17"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="53" t="s">
+      <c r="L11" s="52"/>
+      <c r="M11" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="47"/>
       <c r="Q11" s="6"/>
       <c r="U11" s="35" t="s">
         <v>6</v>
@@ -1320,11 +1320,11 @@
       </c>
       <c r="J12" s="20"/>
       <c r="K12" s="39"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="48"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="49"/>
       <c r="Q12" s="6"/>
       <c r="U12" s="35" t="s">
         <v>18</v>
@@ -1344,7 +1344,7 @@
       <c r="I13" s="36"/>
       <c r="J13" s="36"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="52"/>
+      <c r="L13" s="53"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="6"/>
@@ -1363,20 +1363,20 @@
     </row>
     <row r="14" spans="6:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="4"/>
-      <c r="G14" s="55" t="s">
+      <c r="G14" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="45" t="s">
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="47"/>
       <c r="Q14" s="6"/>
       <c r="U14" s="35" t="s">
         <v>20</v>
@@ -1397,16 +1397,16 @@
     </row>
     <row r="15" spans="6:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F15" s="4"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="48"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="49"/>
       <c r="Q15" s="6"/>
       <c r="U15" s="35" t="s">
         <v>1</v>

</xml_diff>